<commit_message>
Atualizado por script em 29-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/brazil_serie-a_2023.xlsx
+++ b/2023/brazil_serie-a_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V351"/>
+  <dimension ref="A1:V352"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -941,7 +941,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Athletico-PR</t>
+          <t>Botafogo RJ</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -949,63 +949,63 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Goias</t>
+          <t>Sao Paulo</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>1.64</v>
+        <v>2.69</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>09/04/2023 08:36</t>
+          <t>08/04/2023 23:42</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>1.64</v>
+        <v>2.46</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>15/04/2023 23:27</t>
+          <t>15/04/2023 23:22</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>4.15</v>
+        <v>3.05</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>09/04/2023 08:36</t>
+          <t>08/04/2023 23:42</t>
         </is>
       </c>
       <c r="P6" t="n">
-        <v>3.69</v>
+        <v>3.17</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>15/04/2023 23:27</t>
+          <t>15/04/2023 23:25</t>
         </is>
       </c>
       <c r="R6" t="n">
-        <v>5.21</v>
+        <v>3</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>09/04/2023 08:36</t>
+          <t>08/04/2023 23:42</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>6.64</v>
+        <v>3.26</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>15/04/2023 23:28</t>
+          <t>15/04/2023 23:25</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/athletico-pr-goias/Sv02EkgD/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/botafogo-rj-sao-paulo/vFRENgWQ/</t>
         </is>
       </c>
     </row>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Botafogo RJ</t>
+          <t>Athletico-PR</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -1041,63 +1041,63 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Sao Paulo</t>
+          <t>Goias</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>2.69</v>
+        <v>1.64</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>08/04/2023 23:42</t>
+          <t>09/04/2023 08:36</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>2.46</v>
+        <v>1.64</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>15/04/2023 23:22</t>
+          <t>15/04/2023 23:27</t>
         </is>
       </c>
       <c r="N7" t="n">
-        <v>3.05</v>
+        <v>4.15</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>08/04/2023 23:42</t>
+          <t>09/04/2023 08:36</t>
         </is>
       </c>
       <c r="P7" t="n">
-        <v>3.17</v>
+        <v>3.69</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>15/04/2023 23:25</t>
+          <t>15/04/2023 23:27</t>
         </is>
       </c>
       <c r="R7" t="n">
-        <v>3</v>
+        <v>5.21</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>08/04/2023 23:42</t>
+          <t>09/04/2023 08:36</t>
         </is>
       </c>
       <c r="T7" t="n">
-        <v>3.26</v>
+        <v>6.64</v>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>15/04/2023 23:25</t>
+          <t>15/04/2023 23:28</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/botafogo-rj-sao-paulo/vFRENgWQ/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/athletico-pr-goias/Sv02EkgD/</t>
         </is>
       </c>
     </row>
@@ -2413,71 +2413,71 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Coritiba</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Fluminense</t>
+          <t>Sao Paulo</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J22" t="n">
-        <v>2.69</v>
+        <v>3.08</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>24/04/2023 05:12</t>
+          <t>23/04/2023 23:42</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>2.16</v>
+        <v>3.03</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>29/04/2023 21:29</t>
+          <t>29/04/2023 21:23</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.27</v>
+        <v>3.36</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>24/04/2023 05:12</t>
+          <t>23/04/2023 23:42</t>
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.34</v>
+        <v>3.18</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>29/04/2023 21:29</t>
+          <t>29/04/2023 21:16</t>
         </is>
       </c>
       <c r="R22" t="n">
-        <v>2.77</v>
+        <v>2.4</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>24/04/2023 05:12</t>
+          <t>23/04/2023 23:42</t>
         </is>
       </c>
       <c r="T22" t="n">
-        <v>3.76</v>
+        <v>2.61</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>29/04/2023 21:29</t>
+          <t>29/04/2023 21:23</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/fortaleza-fluminense/Q7RQo3Eo/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/coritiba-sao-paulo/b1wqNJyo/</t>
         </is>
       </c>
     </row>
@@ -2505,71 +2505,71 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Coritiba</t>
+          <t>Fortaleza</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Sao Paulo</t>
+          <t>Fluminense</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J23" t="n">
-        <v>3.08</v>
+        <v>2.69</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>23/04/2023 23:42</t>
+          <t>24/04/2023 05:12</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>3.03</v>
+        <v>2.16</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>29/04/2023 21:23</t>
+          <t>29/04/2023 21:29</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>3.36</v>
+        <v>3.27</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>23/04/2023 23:42</t>
+          <t>24/04/2023 05:12</t>
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3.18</v>
+        <v>3.34</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>29/04/2023 21:16</t>
+          <t>29/04/2023 21:29</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>2.4</v>
+        <v>2.77</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>23/04/2023 23:42</t>
+          <t>24/04/2023 05:12</t>
         </is>
       </c>
       <c r="T23" t="n">
-        <v>2.61</v>
+        <v>3.76</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>29/04/2023 21:23</t>
+          <t>29/04/2023 21:29</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/coritiba-sao-paulo/b1wqNJyo/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/fortaleza-fluminense/Q7RQo3Eo/</t>
         </is>
       </c>
     </row>
@@ -19709,71 +19709,71 @@
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>Athletico-PR</t>
+          <t>Goias</t>
         </is>
       </c>
       <c r="G210" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>Atletico-MG</t>
+          <t>Internacional</t>
         </is>
       </c>
       <c r="I210" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J210" t="n">
-        <v>2.29</v>
+        <v>2.65</v>
       </c>
       <c r="K210" t="inlineStr">
         <is>
-          <t>27/08/2023 22:42</t>
+          <t>27/08/2023 01:12</t>
         </is>
       </c>
       <c r="L210" t="n">
-        <v>2.46</v>
+        <v>2.9</v>
       </c>
       <c r="M210" t="inlineStr">
         <is>
-          <t>02/09/2023 20:59</t>
+          <t>02/09/2023 20:51</t>
         </is>
       </c>
       <c r="N210" t="n">
-        <v>3.1</v>
+        <v>3.06</v>
       </c>
       <c r="O210" t="inlineStr">
         <is>
-          <t>27/08/2023 22:42</t>
+          <t>27/08/2023 01:12</t>
         </is>
       </c>
       <c r="P210" t="n">
+        <v>2.89</v>
+      </c>
+      <c r="Q210" t="inlineStr">
+        <is>
+          <t>02/09/2023 20:51</t>
+        </is>
+      </c>
+      <c r="R210" t="n">
         <v>3.06</v>
       </c>
-      <c r="Q210" t="inlineStr">
-        <is>
-          <t>02/09/2023 20:55</t>
-        </is>
-      </c>
-      <c r="R210" t="n">
-        <v>3.58</v>
-      </c>
       <c r="S210" t="inlineStr">
         <is>
-          <t>27/08/2023 22:42</t>
+          <t>27/08/2023 01:12</t>
         </is>
       </c>
       <c r="T210" t="n">
-        <v>3.41</v>
+        <v>2.97</v>
       </c>
       <c r="U210" t="inlineStr">
         <is>
-          <t>02/09/2023 20:59</t>
+          <t>02/09/2023 20:51</t>
         </is>
       </c>
       <c r="V210" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/athletico-pr-atletico-mg/2quwqVYp/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/goias-internacional/fwj3kXeH/</t>
         </is>
       </c>
     </row>
@@ -19801,71 +19801,71 @@
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>Goias</t>
+          <t>Athletico-PR</t>
         </is>
       </c>
       <c r="G211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>Internacional</t>
+          <t>Atletico-MG</t>
         </is>
       </c>
       <c r="I211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J211" t="n">
-        <v>2.65</v>
+        <v>2.29</v>
       </c>
       <c r="K211" t="inlineStr">
         <is>
-          <t>27/08/2023 01:12</t>
+          <t>27/08/2023 22:42</t>
         </is>
       </c>
       <c r="L211" t="n">
-        <v>2.9</v>
+        <v>2.46</v>
       </c>
       <c r="M211" t="inlineStr">
         <is>
-          <t>02/09/2023 20:51</t>
+          <t>02/09/2023 20:59</t>
         </is>
       </c>
       <c r="N211" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="O211" t="inlineStr">
+        <is>
+          <t>27/08/2023 22:42</t>
+        </is>
+      </c>
+      <c r="P211" t="n">
         <v>3.06</v>
       </c>
-      <c r="O211" t="inlineStr">
-        <is>
-          <t>27/08/2023 01:12</t>
-        </is>
-      </c>
-      <c r="P211" t="n">
-        <v>2.89</v>
-      </c>
       <c r="Q211" t="inlineStr">
         <is>
-          <t>02/09/2023 20:51</t>
+          <t>02/09/2023 20:55</t>
         </is>
       </c>
       <c r="R211" t="n">
-        <v>3.06</v>
+        <v>3.58</v>
       </c>
       <c r="S211" t="inlineStr">
         <is>
-          <t>27/08/2023 01:12</t>
+          <t>27/08/2023 22:42</t>
         </is>
       </c>
       <c r="T211" t="n">
-        <v>2.97</v>
+        <v>3.41</v>
       </c>
       <c r="U211" t="inlineStr">
         <is>
-          <t>02/09/2023 20:51</t>
+          <t>02/09/2023 20:59</t>
         </is>
       </c>
       <c r="V211" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/goias-internacional/fwj3kXeH/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/athletico-pr-atletico-mg/2quwqVYp/</t>
         </is>
       </c>
     </row>
@@ -20537,62 +20537,62 @@
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>Flamengo RJ</t>
+          <t>Internacional</t>
         </is>
       </c>
       <c r="G219" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H219" t="inlineStr">
         <is>
-          <t>Athletico-PR</t>
+          <t>Sao Paulo</t>
         </is>
       </c>
       <c r="I219" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J219" t="n">
-        <v>1.72</v>
+        <v>2.35</v>
       </c>
       <c r="K219" t="inlineStr">
         <is>
-          <t>04/09/2023 08:42</t>
+          <t>04/09/2023 18:12</t>
         </is>
       </c>
       <c r="L219" t="n">
-        <v>1.81</v>
+        <v>2.71</v>
       </c>
       <c r="M219" t="inlineStr">
         <is>
+          <t>14/09/2023 02:29</t>
+        </is>
+      </c>
+      <c r="N219" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="O219" t="inlineStr">
+        <is>
+          <t>04/09/2023 18:12</t>
+        </is>
+      </c>
+      <c r="P219" t="n">
+        <v>3.06</v>
+      </c>
+      <c r="Q219" t="inlineStr">
+        <is>
           <t>14/09/2023 02:21</t>
         </is>
       </c>
-      <c r="N219" t="n">
-        <v>3.99</v>
-      </c>
-      <c r="O219" t="inlineStr">
-        <is>
-          <t>04/09/2023 08:42</t>
-        </is>
-      </c>
-      <c r="P219" t="n">
-        <v>3.58</v>
-      </c>
-      <c r="Q219" t="inlineStr">
-        <is>
-          <t>14/09/2023 02:22</t>
-        </is>
-      </c>
       <c r="R219" t="n">
-        <v>4.75</v>
+        <v>3.38</v>
       </c>
       <c r="S219" t="inlineStr">
         <is>
-          <t>04/09/2023 08:42</t>
+          <t>04/09/2023 18:12</t>
         </is>
       </c>
       <c r="T219" t="n">
-        <v>5.02</v>
+        <v>3.01</v>
       </c>
       <c r="U219" t="inlineStr">
         <is>
@@ -20601,7 +20601,7 @@
       </c>
       <c r="V219" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/flamengo-rj-athletico-pr/CEMT5htb/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/internacional-sao-paulo/bVhBq2Pe/</t>
         </is>
       </c>
     </row>
@@ -20629,71 +20629,71 @@
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>Internacional</t>
+          <t>Flamengo RJ</t>
         </is>
       </c>
       <c r="G220" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H220" t="inlineStr">
         <is>
-          <t>Sao Paulo</t>
+          <t>Athletico-PR</t>
         </is>
       </c>
       <c r="I220" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J220" t="n">
-        <v>2.35</v>
+        <v>1.72</v>
       </c>
       <c r="K220" t="inlineStr">
         <is>
-          <t>04/09/2023 18:12</t>
+          <t>04/09/2023 08:42</t>
         </is>
       </c>
       <c r="L220" t="n">
-        <v>2.71</v>
+        <v>1.81</v>
       </c>
       <c r="M220" t="inlineStr">
         <is>
+          <t>14/09/2023 02:21</t>
+        </is>
+      </c>
+      <c r="N220" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="O220" t="inlineStr">
+        <is>
+          <t>04/09/2023 08:42</t>
+        </is>
+      </c>
+      <c r="P220" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="Q220" t="inlineStr">
+        <is>
+          <t>14/09/2023 02:22</t>
+        </is>
+      </c>
+      <c r="R220" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="S220" t="inlineStr">
+        <is>
+          <t>04/09/2023 08:42</t>
+        </is>
+      </c>
+      <c r="T220" t="n">
+        <v>5.02</v>
+      </c>
+      <c r="U220" t="inlineStr">
+        <is>
           <t>14/09/2023 02:29</t>
         </is>
       </c>
-      <c r="N220" t="n">
-        <v>3.16</v>
-      </c>
-      <c r="O220" t="inlineStr">
-        <is>
-          <t>04/09/2023 18:12</t>
-        </is>
-      </c>
-      <c r="P220" t="n">
-        <v>3.06</v>
-      </c>
-      <c r="Q220" t="inlineStr">
-        <is>
-          <t>14/09/2023 02:21</t>
-        </is>
-      </c>
-      <c r="R220" t="n">
-        <v>3.38</v>
-      </c>
-      <c r="S220" t="inlineStr">
-        <is>
-          <t>04/09/2023 18:12</t>
-        </is>
-      </c>
-      <c r="T220" t="n">
-        <v>3.01</v>
-      </c>
-      <c r="U220" t="inlineStr">
-        <is>
-          <t>14/09/2023 02:29</t>
-        </is>
-      </c>
       <c r="V220" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/internacional-sao-paulo/bVhBq2Pe/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/flamengo-rj-athletico-pr/CEMT5htb/</t>
         </is>
       </c>
     </row>
@@ -22837,71 +22837,71 @@
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Sao Paulo</t>
         </is>
       </c>
       <c r="G244" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>Fluminense</t>
+          <t>Corinthians</t>
         </is>
       </c>
       <c r="I244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J244" t="n">
-        <v>2.64</v>
+        <v>1.64</v>
       </c>
       <c r="K244" t="inlineStr">
         <is>
-          <t>24/09/2023 01:12</t>
+          <t>27/09/2023 23:12</t>
         </is>
       </c>
       <c r="L244" t="n">
-        <v>2.33</v>
+        <v>1.52</v>
       </c>
       <c r="M244" t="inlineStr">
         <is>
-          <t>30/09/2023 23:04</t>
+          <t>30/09/2023 23:20</t>
         </is>
       </c>
       <c r="N244" t="n">
-        <v>3.09</v>
+        <v>3.73</v>
       </c>
       <c r="O244" t="inlineStr">
         <is>
-          <t>24/09/2023 01:12</t>
+          <t>27/09/2023 23:12</t>
         </is>
       </c>
       <c r="P244" t="n">
-        <v>3.1</v>
+        <v>3.96</v>
       </c>
       <c r="Q244" t="inlineStr">
         <is>
-          <t>30/09/2023 23:04</t>
+          <t>30/09/2023 23:26</t>
         </is>
       </c>
       <c r="R244" t="n">
-        <v>3.04</v>
+        <v>6.33</v>
       </c>
       <c r="S244" t="inlineStr">
         <is>
-          <t>24/09/2023 01:12</t>
+          <t>27/09/2023 23:12</t>
         </is>
       </c>
       <c r="T244" t="n">
-        <v>3.62</v>
+        <v>8.24</v>
       </c>
       <c r="U244" t="inlineStr">
         <is>
-          <t>30/09/2023 23:04</t>
+          <t>30/09/2023 23:28</t>
         </is>
       </c>
       <c r="V244" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/cuiaba-fluminense/hWWPVu0K/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/sao-paulo-corinthians/v3gJC0gr/</t>
         </is>
       </c>
     </row>
@@ -22929,71 +22929,71 @@
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>Sao Paulo</t>
+          <t>Cuiaba</t>
         </is>
       </c>
       <c r="G245" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H245" t="inlineStr">
         <is>
-          <t>Corinthians</t>
+          <t>Fluminense</t>
         </is>
       </c>
       <c r="I245" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J245" t="n">
-        <v>1.64</v>
+        <v>2.64</v>
       </c>
       <c r="K245" t="inlineStr">
         <is>
-          <t>27/09/2023 23:12</t>
+          <t>24/09/2023 01:12</t>
         </is>
       </c>
       <c r="L245" t="n">
-        <v>1.52</v>
+        <v>2.33</v>
       </c>
       <c r="M245" t="inlineStr">
         <is>
-          <t>30/09/2023 23:20</t>
+          <t>30/09/2023 23:04</t>
         </is>
       </c>
       <c r="N245" t="n">
-        <v>3.73</v>
+        <v>3.09</v>
       </c>
       <c r="O245" t="inlineStr">
         <is>
-          <t>27/09/2023 23:12</t>
+          <t>24/09/2023 01:12</t>
         </is>
       </c>
       <c r="P245" t="n">
-        <v>3.96</v>
+        <v>3.1</v>
       </c>
       <c r="Q245" t="inlineStr">
         <is>
-          <t>30/09/2023 23:26</t>
+          <t>30/09/2023 23:04</t>
         </is>
       </c>
       <c r="R245" t="n">
-        <v>6.33</v>
+        <v>3.04</v>
       </c>
       <c r="S245" t="inlineStr">
         <is>
-          <t>27/09/2023 23:12</t>
+          <t>24/09/2023 01:12</t>
         </is>
       </c>
       <c r="T245" t="n">
-        <v>8.24</v>
+        <v>3.62</v>
       </c>
       <c r="U245" t="inlineStr">
         <is>
-          <t>30/09/2023 23:28</t>
+          <t>30/09/2023 23:04</t>
         </is>
       </c>
       <c r="V245" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/sao-paulo-corinthians/v3gJC0gr/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/cuiaba-fluminense/hWWPVu0K/</t>
         </is>
       </c>
     </row>
@@ -23205,71 +23205,71 @@
       </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t>Santos</t>
+          <t>Coritiba</t>
         </is>
       </c>
       <c r="G248" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H248" t="inlineStr">
         <is>
-          <t>Vasco</t>
+          <t>Athletico-PR</t>
         </is>
       </c>
       <c r="I248" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J248" t="n">
-        <v>2.25</v>
+        <v>3.07</v>
       </c>
       <c r="K248" t="inlineStr">
         <is>
-          <t>26/09/2023 00:12</t>
+          <t>27/09/2023 23:12</t>
         </is>
       </c>
       <c r="L248" t="n">
-        <v>2.6</v>
+        <v>3.68</v>
       </c>
       <c r="M248" t="inlineStr">
         <is>
-          <t>01/10/2023 20:30</t>
+          <t>01/10/2023 20:56</t>
         </is>
       </c>
       <c r="N248" t="n">
-        <v>3.29</v>
+        <v>3.23</v>
       </c>
       <c r="O248" t="inlineStr">
         <is>
-          <t>26/09/2023 00:12</t>
+          <t>27/09/2023 23:12</t>
         </is>
       </c>
       <c r="P248" t="n">
-        <v>3.11</v>
+        <v>3.26</v>
       </c>
       <c r="Q248" t="inlineStr">
         <is>
-          <t>01/10/2023 20:57</t>
+          <t>01/10/2023 20:29</t>
         </is>
       </c>
       <c r="R248" t="n">
-        <v>3.44</v>
+        <v>2.48</v>
       </c>
       <c r="S248" t="inlineStr">
         <is>
-          <t>26/09/2023 00:12</t>
+          <t>27/09/2023 23:12</t>
         </is>
       </c>
       <c r="T248" t="n">
-        <v>3.11</v>
+        <v>2.22</v>
       </c>
       <c r="U248" t="inlineStr">
         <is>
-          <t>01/10/2023 20:30</t>
+          <t>01/10/2023 20:56</t>
         </is>
       </c>
       <c r="V248" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/santos-vasco/IghNBK8l/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/coritiba-athletico-pr/0xpv8x8D/</t>
         </is>
       </c>
     </row>
@@ -23297,71 +23297,71 @@
       </c>
       <c r="F249" t="inlineStr">
         <is>
-          <t>Coritiba</t>
+          <t>Santos</t>
         </is>
       </c>
       <c r="G249" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>Athletico-PR</t>
+          <t>Vasco</t>
         </is>
       </c>
       <c r="I249" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J249" t="n">
-        <v>3.07</v>
+        <v>2.25</v>
       </c>
       <c r="K249" t="inlineStr">
         <is>
-          <t>27/09/2023 23:12</t>
+          <t>26/09/2023 00:12</t>
         </is>
       </c>
       <c r="L249" t="n">
-        <v>3.68</v>
+        <v>2.6</v>
       </c>
       <c r="M249" t="inlineStr">
         <is>
-          <t>01/10/2023 20:56</t>
+          <t>01/10/2023 20:30</t>
         </is>
       </c>
       <c r="N249" t="n">
-        <v>3.23</v>
+        <v>3.29</v>
       </c>
       <c r="O249" t="inlineStr">
         <is>
-          <t>27/09/2023 23:12</t>
+          <t>26/09/2023 00:12</t>
         </is>
       </c>
       <c r="P249" t="n">
-        <v>3.26</v>
+        <v>3.11</v>
       </c>
       <c r="Q249" t="inlineStr">
         <is>
-          <t>01/10/2023 20:29</t>
+          <t>01/10/2023 20:57</t>
         </is>
       </c>
       <c r="R249" t="n">
-        <v>2.48</v>
+        <v>3.44</v>
       </c>
       <c r="S249" t="inlineStr">
         <is>
-          <t>27/09/2023 23:12</t>
+          <t>26/09/2023 00:12</t>
         </is>
       </c>
       <c r="T249" t="n">
-        <v>2.22</v>
+        <v>3.11</v>
       </c>
       <c r="U249" t="inlineStr">
         <is>
-          <t>01/10/2023 20:56</t>
+          <t>01/10/2023 20:30</t>
         </is>
       </c>
       <c r="V249" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/coritiba-athletico-pr/0xpv8x8D/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/santos-vasco/IghNBK8l/</t>
         </is>
       </c>
     </row>
@@ -24125,71 +24125,71 @@
       </c>
       <c r="F258" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Athletico-PR</t>
         </is>
       </c>
       <c r="G258" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>America MG</t>
+          <t>Bragantino</t>
         </is>
       </c>
       <c r="I258" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J258" t="n">
-        <v>1.57</v>
+        <v>2.09</v>
       </c>
       <c r="K258" t="inlineStr">
         <is>
-          <t>01/10/2023 20:12</t>
+          <t>01/10/2023 22:42</t>
         </is>
       </c>
       <c r="L258" t="n">
-        <v>1.53</v>
+        <v>2.76</v>
       </c>
       <c r="M258" t="inlineStr">
         <is>
-          <t>08/10/2023 22:46</t>
+          <t>08/10/2023 23:26</t>
         </is>
       </c>
       <c r="N258" t="n">
-        <v>4.3</v>
+        <v>3.44</v>
       </c>
       <c r="O258" t="inlineStr">
         <is>
-          <t>01/10/2023 20:12</t>
+          <t>01/10/2023 22:42</t>
         </is>
       </c>
       <c r="P258" t="n">
-        <v>4.43</v>
+        <v>3.22</v>
       </c>
       <c r="Q258" t="inlineStr">
         <is>
-          <t>08/10/2023 23:29</t>
+          <t>08/10/2023 23:26</t>
         </is>
       </c>
       <c r="R258" t="n">
-        <v>5.96</v>
+        <v>3.7</v>
       </c>
       <c r="S258" t="inlineStr">
         <is>
-          <t>01/10/2023 20:12</t>
+          <t>01/10/2023 22:42</t>
         </is>
       </c>
       <c r="T258" t="n">
-        <v>6.46</v>
+        <v>2.82</v>
       </c>
       <c r="U258" t="inlineStr">
         <is>
-          <t>08/10/2023 23:29</t>
+          <t>08/10/2023 23:26</t>
         </is>
       </c>
       <c r="V258" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/fortaleza-america-mg/lbn4qaUJ/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/athletico-pr-bragantino/ng8LKFiJ/</t>
         </is>
       </c>
     </row>
@@ -24217,7 +24217,7 @@
       </c>
       <c r="F259" t="inlineStr">
         <is>
-          <t>Athletico-PR</t>
+          <t>Atletico-MG</t>
         </is>
       </c>
       <c r="G259" t="n">
@@ -24225,63 +24225,63 @@
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>Bragantino</t>
+          <t>Coritiba</t>
         </is>
       </c>
       <c r="I259" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J259" t="n">
-        <v>2.09</v>
+        <v>1.35</v>
       </c>
       <c r="K259" t="inlineStr">
         <is>
-          <t>01/10/2023 22:42</t>
+          <t>01/10/2023 20:12</t>
         </is>
       </c>
       <c r="L259" t="n">
-        <v>2.76</v>
+        <v>1.39</v>
       </c>
       <c r="M259" t="inlineStr">
         <is>
-          <t>08/10/2023 23:26</t>
+          <t>08/10/2023 23:23</t>
         </is>
       </c>
       <c r="N259" t="n">
-        <v>3.44</v>
+        <v>4.9</v>
       </c>
       <c r="O259" t="inlineStr">
         <is>
-          <t>01/10/2023 22:42</t>
+          <t>01/10/2023 20:12</t>
         </is>
       </c>
       <c r="P259" t="n">
-        <v>3.22</v>
+        <v>4.75</v>
       </c>
       <c r="Q259" t="inlineStr">
         <is>
-          <t>08/10/2023 23:26</t>
+          <t>08/10/2023 23:23</t>
         </is>
       </c>
       <c r="R259" t="n">
-        <v>3.7</v>
+        <v>10.08</v>
       </c>
       <c r="S259" t="inlineStr">
         <is>
-          <t>01/10/2023 22:42</t>
+          <t>01/10/2023 20:12</t>
         </is>
       </c>
       <c r="T259" t="n">
-        <v>2.82</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="U259" t="inlineStr">
         <is>
-          <t>08/10/2023 23:26</t>
+          <t>08/10/2023 23:25</t>
         </is>
       </c>
       <c r="V259" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/athletico-pr-bragantino/ng8LKFiJ/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/atletico-mg-coritiba/vT4DMyN6/</t>
         </is>
       </c>
     </row>
@@ -24309,22 +24309,22 @@
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>Atletico-MG</t>
+          <t>Fortaleza</t>
         </is>
       </c>
       <c r="G260" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H260" t="inlineStr">
         <is>
-          <t>Coritiba</t>
+          <t>America MG</t>
         </is>
       </c>
       <c r="I260" t="n">
         <v>2</v>
       </c>
       <c r="J260" t="n">
-        <v>1.35</v>
+        <v>1.57</v>
       </c>
       <c r="K260" t="inlineStr">
         <is>
@@ -24332,15 +24332,15 @@
         </is>
       </c>
       <c r="L260" t="n">
-        <v>1.39</v>
+        <v>1.53</v>
       </c>
       <c r="M260" t="inlineStr">
         <is>
-          <t>08/10/2023 23:23</t>
+          <t>08/10/2023 22:46</t>
         </is>
       </c>
       <c r="N260" t="n">
-        <v>4.9</v>
+        <v>4.3</v>
       </c>
       <c r="O260" t="inlineStr">
         <is>
@@ -24348,15 +24348,15 @@
         </is>
       </c>
       <c r="P260" t="n">
-        <v>4.75</v>
+        <v>4.43</v>
       </c>
       <c r="Q260" t="inlineStr">
         <is>
-          <t>08/10/2023 23:23</t>
+          <t>08/10/2023 23:29</t>
         </is>
       </c>
       <c r="R260" t="n">
-        <v>10.08</v>
+        <v>5.96</v>
       </c>
       <c r="S260" t="inlineStr">
         <is>
@@ -24364,16 +24364,16 @@
         </is>
       </c>
       <c r="T260" t="n">
-        <v>9.800000000000001</v>
+        <v>6.46</v>
       </c>
       <c r="U260" t="inlineStr">
         <is>
-          <t>08/10/2023 23:25</t>
+          <t>08/10/2023 23:29</t>
         </is>
       </c>
       <c r="V260" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/atletico-mg-coritiba/vT4DMyN6/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/fortaleza-america-mg/lbn4qaUJ/</t>
         </is>
       </c>
     </row>
@@ -24769,22 +24769,22 @@
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Goias</t>
         </is>
       </c>
       <c r="G265" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H265" t="inlineStr">
         <is>
-          <t>Internacional</t>
+          <t>Sao Paulo</t>
         </is>
       </c>
       <c r="I265" t="n">
         <v>0</v>
       </c>
       <c r="J265" t="n">
-        <v>2.23</v>
+        <v>3.02</v>
       </c>
       <c r="K265" t="inlineStr">
         <is>
@@ -24792,15 +24792,15 @@
         </is>
       </c>
       <c r="L265" t="n">
-        <v>2.07</v>
+        <v>3.79</v>
       </c>
       <c r="M265" t="inlineStr">
         <is>
-          <t>19/10/2023 02:29</t>
+          <t>19/10/2023 02:27</t>
         </is>
       </c>
       <c r="N265" t="n">
-        <v>3.32</v>
+        <v>3.09</v>
       </c>
       <c r="O265" t="inlineStr">
         <is>
@@ -24808,15 +24808,15 @@
         </is>
       </c>
       <c r="P265" t="n">
-        <v>3.37</v>
+        <v>3.19</v>
       </c>
       <c r="Q265" t="inlineStr">
         <is>
-          <t>19/10/2023 02:21</t>
+          <t>19/10/2023 02:27</t>
         </is>
       </c>
       <c r="R265" t="n">
-        <v>3.54</v>
+        <v>2.66</v>
       </c>
       <c r="S265" t="inlineStr">
         <is>
@@ -24824,16 +24824,16 @@
         </is>
       </c>
       <c r="T265" t="n">
-        <v>4.04</v>
+        <v>2.22</v>
       </c>
       <c r="U265" t="inlineStr">
         <is>
-          <t>19/10/2023 02:29</t>
+          <t>19/10/2023 02:27</t>
         </is>
       </c>
       <c r="V265" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/bahia-internacional/KEG2ujTo/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/goias-sao-paulo/b76rzei6/</t>
         </is>
       </c>
     </row>
@@ -24861,22 +24861,22 @@
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>Goias</t>
+          <t>Bahia</t>
         </is>
       </c>
       <c r="G266" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H266" t="inlineStr">
         <is>
-          <t>Sao Paulo</t>
+          <t>Internacional</t>
         </is>
       </c>
       <c r="I266" t="n">
         <v>0</v>
       </c>
       <c r="J266" t="n">
-        <v>3.02</v>
+        <v>2.23</v>
       </c>
       <c r="K266" t="inlineStr">
         <is>
@@ -24884,15 +24884,15 @@
         </is>
       </c>
       <c r="L266" t="n">
-        <v>3.79</v>
+        <v>2.07</v>
       </c>
       <c r="M266" t="inlineStr">
         <is>
-          <t>19/10/2023 02:27</t>
+          <t>19/10/2023 02:29</t>
         </is>
       </c>
       <c r="N266" t="n">
-        <v>3.09</v>
+        <v>3.32</v>
       </c>
       <c r="O266" t="inlineStr">
         <is>
@@ -24900,15 +24900,15 @@
         </is>
       </c>
       <c r="P266" t="n">
-        <v>3.19</v>
+        <v>3.37</v>
       </c>
       <c r="Q266" t="inlineStr">
         <is>
-          <t>19/10/2023 02:27</t>
+          <t>19/10/2023 02:21</t>
         </is>
       </c>
       <c r="R266" t="n">
-        <v>2.66</v>
+        <v>3.54</v>
       </c>
       <c r="S266" t="inlineStr">
         <is>
@@ -24916,16 +24916,16 @@
         </is>
       </c>
       <c r="T266" t="n">
-        <v>2.22</v>
+        <v>4.04</v>
       </c>
       <c r="U266" t="inlineStr">
         <is>
-          <t>19/10/2023 02:27</t>
+          <t>19/10/2023 02:29</t>
         </is>
       </c>
       <c r="V266" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/goias-sao-paulo/b76rzei6/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/bahia-internacional/KEG2ujTo/</t>
         </is>
       </c>
     </row>
@@ -25413,22 +25413,22 @@
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Cuiaba</t>
         </is>
       </c>
       <c r="G272" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H272" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Goias</t>
         </is>
       </c>
       <c r="I272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J272" t="n">
-        <v>2.3</v>
+        <v>1.81</v>
       </c>
       <c r="K272" t="inlineStr">
         <is>
@@ -25436,15 +25436,15 @@
         </is>
       </c>
       <c r="L272" t="n">
-        <v>2.09</v>
+        <v>2.05</v>
       </c>
       <c r="M272" t="inlineStr">
         <is>
-          <t>21/10/2023 23:22</t>
+          <t>21/10/2023 23:28</t>
         </is>
       </c>
       <c r="N272" t="n">
-        <v>3.33</v>
+        <v>3.48</v>
       </c>
       <c r="O272" t="inlineStr">
         <is>
@@ -25452,15 +25452,15 @@
         </is>
       </c>
       <c r="P272" t="n">
-        <v>3.39</v>
+        <v>3.18</v>
       </c>
       <c r="Q272" t="inlineStr">
         <is>
-          <t>21/10/2023 23:18</t>
+          <t>21/10/2023 23:28</t>
         </is>
       </c>
       <c r="R272" t="n">
-        <v>3.36</v>
+        <v>4.93</v>
       </c>
       <c r="S272" t="inlineStr">
         <is>
@@ -25468,16 +25468,16 @@
         </is>
       </c>
       <c r="T272" t="n">
-        <v>3.93</v>
+        <v>4.4</v>
       </c>
       <c r="U272" t="inlineStr">
         <is>
-          <t>21/10/2023 23:22</t>
+          <t>21/10/2023 23:28</t>
         </is>
       </c>
       <c r="V272" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/bahia-fortaleza/d0Hrxxvi/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/cuiaba-goias/ziGnydgc/</t>
         </is>
       </c>
     </row>
@@ -25505,22 +25505,22 @@
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Bahia</t>
         </is>
       </c>
       <c r="G273" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H273" t="inlineStr">
         <is>
-          <t>Goias</t>
+          <t>Fortaleza</t>
         </is>
       </c>
       <c r="I273" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J273" t="n">
-        <v>1.81</v>
+        <v>2.3</v>
       </c>
       <c r="K273" t="inlineStr">
         <is>
@@ -25528,15 +25528,15 @@
         </is>
       </c>
       <c r="L273" t="n">
-        <v>2.05</v>
+        <v>2.09</v>
       </c>
       <c r="M273" t="inlineStr">
         <is>
-          <t>21/10/2023 23:28</t>
+          <t>21/10/2023 23:22</t>
         </is>
       </c>
       <c r="N273" t="n">
-        <v>3.48</v>
+        <v>3.33</v>
       </c>
       <c r="O273" t="inlineStr">
         <is>
@@ -25544,15 +25544,15 @@
         </is>
       </c>
       <c r="P273" t="n">
-        <v>3.18</v>
+        <v>3.39</v>
       </c>
       <c r="Q273" t="inlineStr">
         <is>
-          <t>21/10/2023 23:28</t>
+          <t>21/10/2023 23:18</t>
         </is>
       </c>
       <c r="R273" t="n">
-        <v>4.93</v>
+        <v>3.36</v>
       </c>
       <c r="S273" t="inlineStr">
         <is>
@@ -25560,16 +25560,16 @@
         </is>
       </c>
       <c r="T273" t="n">
-        <v>4.4</v>
+        <v>3.93</v>
       </c>
       <c r="U273" t="inlineStr">
         <is>
-          <t>21/10/2023 23:28</t>
+          <t>21/10/2023 23:22</t>
         </is>
       </c>
       <c r="V273" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/cuiaba-goias/ziGnydgc/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/bahia-fortaleza/d0Hrxxvi/</t>
         </is>
       </c>
     </row>
@@ -25781,71 +25781,71 @@
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>Internacional</t>
+          <t>Atletico-MG</t>
         </is>
       </c>
       <c r="G276" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H276" t="inlineStr">
         <is>
-          <t>Santos</t>
+          <t>Cruzeiro</t>
         </is>
       </c>
       <c r="I276" t="n">
         <v>1</v>
       </c>
       <c r="J276" t="n">
-        <v>1.8</v>
+        <v>1.75</v>
       </c>
       <c r="K276" t="inlineStr">
         <is>
-          <t>20/10/2023 00:12</t>
+          <t>19/10/2023 23:12</t>
         </is>
       </c>
       <c r="L276" t="n">
-        <v>1.54</v>
+        <v>1.92</v>
       </c>
       <c r="M276" t="inlineStr">
         <is>
-          <t>22/10/2023 20:51</t>
+          <t>22/10/2023 20:52</t>
         </is>
       </c>
       <c r="N276" t="n">
-        <v>3.54</v>
+        <v>3.66</v>
       </c>
       <c r="O276" t="inlineStr">
         <is>
-          <t>20/10/2023 00:12</t>
+          <t>19/10/2023 23:12</t>
         </is>
       </c>
       <c r="P276" t="n">
-        <v>4.08</v>
+        <v>3.17</v>
       </c>
       <c r="Q276" t="inlineStr">
         <is>
-          <t>22/10/2023 20:55</t>
+          <t>22/10/2023 20:52</t>
         </is>
       </c>
       <c r="R276" t="n">
-        <v>5.08</v>
+        <v>5.43</v>
       </c>
       <c r="S276" t="inlineStr">
         <is>
-          <t>20/10/2023 00:12</t>
+          <t>19/10/2023 23:12</t>
         </is>
       </c>
       <c r="T276" t="n">
-        <v>7.28</v>
+        <v>5.2</v>
       </c>
       <c r="U276" t="inlineStr">
         <is>
-          <t>22/10/2023 20:55</t>
+          <t>22/10/2023 20:56</t>
         </is>
       </c>
       <c r="V276" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/internacional-santos/vPnbUPKp/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/atletico-mg-cruzeiro/Mq0WY5CT/</t>
         </is>
       </c>
     </row>
@@ -25965,71 +25965,71 @@
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>Atletico-MG</t>
+          <t>Internacional</t>
         </is>
       </c>
       <c r="G278" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H278" t="inlineStr">
         <is>
-          <t>Cruzeiro</t>
+          <t>Santos</t>
         </is>
       </c>
       <c r="I278" t="n">
         <v>1</v>
       </c>
       <c r="J278" t="n">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="K278" t="inlineStr">
         <is>
-          <t>19/10/2023 23:12</t>
+          <t>20/10/2023 00:12</t>
         </is>
       </c>
       <c r="L278" t="n">
-        <v>1.92</v>
+        <v>1.54</v>
       </c>
       <c r="M278" t="inlineStr">
         <is>
-          <t>22/10/2023 20:52</t>
+          <t>22/10/2023 20:51</t>
         </is>
       </c>
       <c r="N278" t="n">
-        <v>3.66</v>
+        <v>3.54</v>
       </c>
       <c r="O278" t="inlineStr">
         <is>
-          <t>19/10/2023 23:12</t>
+          <t>20/10/2023 00:12</t>
         </is>
       </c>
       <c r="P278" t="n">
-        <v>3.17</v>
+        <v>4.08</v>
       </c>
       <c r="Q278" t="inlineStr">
         <is>
-          <t>22/10/2023 20:52</t>
+          <t>22/10/2023 20:55</t>
         </is>
       </c>
       <c r="R278" t="n">
-        <v>5.43</v>
+        <v>5.08</v>
       </c>
       <c r="S278" t="inlineStr">
         <is>
-          <t>19/10/2023 23:12</t>
+          <t>20/10/2023 00:12</t>
         </is>
       </c>
       <c r="T278" t="n">
-        <v>5.2</v>
+        <v>7.28</v>
       </c>
       <c r="U278" t="inlineStr">
         <is>
-          <t>22/10/2023 20:56</t>
+          <t>22/10/2023 20:55</t>
         </is>
       </c>
       <c r="V278" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/atletico-mg-cruzeiro/Mq0WY5CT/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/internacional-santos/vPnbUPKp/</t>
         </is>
       </c>
     </row>
@@ -26057,71 +26057,71 @@
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>Coritiba</t>
+          <t>Bragantino</t>
         </is>
       </c>
       <c r="G279" t="n">
+        <v>1</v>
+      </c>
+      <c r="H279" t="inlineStr">
+        <is>
+          <t>Fluminense</t>
+        </is>
+      </c>
+      <c r="I279" t="n">
         <v>0</v>
       </c>
-      <c r="H279" t="inlineStr">
-        <is>
-          <t>Palmeiras</t>
-        </is>
-      </c>
-      <c r="I279" t="n">
-        <v>2</v>
-      </c>
       <c r="J279" t="n">
-        <v>4.43</v>
+        <v>1.84</v>
       </c>
       <c r="K279" t="inlineStr">
         <is>
-          <t>19/10/2023 23:13</t>
+          <t>20/10/2023 01:42</t>
         </is>
       </c>
       <c r="L279" t="n">
-        <v>5.19</v>
+        <v>1.76</v>
       </c>
       <c r="M279" t="inlineStr">
         <is>
+          <t>22/10/2023 23:24</t>
+        </is>
+      </c>
+      <c r="N279" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="O279" t="inlineStr">
+        <is>
+          <t>20/10/2023 01:42</t>
+        </is>
+      </c>
+      <c r="P279" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="Q279" t="inlineStr">
+        <is>
+          <t>22/10/2023 23:24</t>
+        </is>
+      </c>
+      <c r="R279" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="S279" t="inlineStr">
+        <is>
+          <t>20/10/2023 01:42</t>
+        </is>
+      </c>
+      <c r="T279" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="U279" t="inlineStr">
+        <is>
           <t>22/10/2023 23:29</t>
         </is>
       </c>
-      <c r="N279" t="n">
-        <v>3.67</v>
-      </c>
-      <c r="O279" t="inlineStr">
-        <is>
-          <t>19/10/2023 23:13</t>
-        </is>
-      </c>
-      <c r="P279" t="n">
-        <v>3.57</v>
-      </c>
-      <c r="Q279" t="inlineStr">
-        <is>
-          <t>22/10/2023 23:27</t>
-        </is>
-      </c>
-      <c r="R279" t="n">
-        <v>1.84</v>
-      </c>
-      <c r="S279" t="inlineStr">
-        <is>
-          <t>19/10/2023 23:13</t>
-        </is>
-      </c>
-      <c r="T279" t="n">
-        <v>1.79</v>
-      </c>
-      <c r="U279" t="inlineStr">
-        <is>
-          <t>22/10/2023 23:29</t>
-        </is>
-      </c>
       <c r="V279" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/coritiba-palmeiras/hSj2Tqzi/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/bragantino-fluminense/rg1SZocN/</t>
         </is>
       </c>
     </row>
@@ -26149,7 +26149,7 @@
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>Bragantino</t>
+          <t>Corinthians</t>
         </is>
       </c>
       <c r="G280" t="n">
@@ -26157,14 +26157,14 @@
       </c>
       <c r="H280" t="inlineStr">
         <is>
-          <t>Fluminense</t>
+          <t>America MG</t>
         </is>
       </c>
       <c r="I280" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J280" t="n">
-        <v>1.84</v>
+        <v>1.75</v>
       </c>
       <c r="K280" t="inlineStr">
         <is>
@@ -26172,15 +26172,15 @@
         </is>
       </c>
       <c r="L280" t="n">
-        <v>1.76</v>
+        <v>2.09</v>
       </c>
       <c r="M280" t="inlineStr">
         <is>
-          <t>22/10/2023 23:24</t>
+          <t>22/10/2023 23:25</t>
         </is>
       </c>
       <c r="N280" t="n">
-        <v>3.7</v>
+        <v>3.78</v>
       </c>
       <c r="O280" t="inlineStr">
         <is>
@@ -26188,15 +26188,15 @@
         </is>
       </c>
       <c r="P280" t="n">
-        <v>3.9</v>
+        <v>3.29</v>
       </c>
       <c r="Q280" t="inlineStr">
         <is>
-          <t>22/10/2023 23:24</t>
+          <t>22/10/2023 23:27</t>
         </is>
       </c>
       <c r="R280" t="n">
-        <v>4.55</v>
+        <v>5.03</v>
       </c>
       <c r="S280" t="inlineStr">
         <is>
@@ -26204,7 +26204,7 @@
         </is>
       </c>
       <c r="T280" t="n">
-        <v>4.85</v>
+        <v>4.08</v>
       </c>
       <c r="U280" t="inlineStr">
         <is>
@@ -26213,7 +26213,7 @@
       </c>
       <c r="V280" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/bragantino-fluminense/rg1SZocN/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/corinthians-america-mg/QH6NzSsH/</t>
         </is>
       </c>
     </row>
@@ -26241,46 +26241,46 @@
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>Corinthians</t>
+          <t>Coritiba</t>
         </is>
       </c>
       <c r="G281" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H281" t="inlineStr">
         <is>
-          <t>America MG</t>
+          <t>Palmeiras</t>
         </is>
       </c>
       <c r="I281" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J281" t="n">
-        <v>1.75</v>
+        <v>4.43</v>
       </c>
       <c r="K281" t="inlineStr">
         <is>
-          <t>20/10/2023 01:42</t>
+          <t>19/10/2023 23:13</t>
         </is>
       </c>
       <c r="L281" t="n">
-        <v>2.09</v>
+        <v>5.19</v>
       </c>
       <c r="M281" t="inlineStr">
         <is>
-          <t>22/10/2023 23:25</t>
+          <t>22/10/2023 23:29</t>
         </is>
       </c>
       <c r="N281" t="n">
-        <v>3.78</v>
+        <v>3.67</v>
       </c>
       <c r="O281" t="inlineStr">
         <is>
-          <t>20/10/2023 01:42</t>
+          <t>19/10/2023 23:13</t>
         </is>
       </c>
       <c r="P281" t="n">
-        <v>3.29</v>
+        <v>3.57</v>
       </c>
       <c r="Q281" t="inlineStr">
         <is>
@@ -26288,15 +26288,15 @@
         </is>
       </c>
       <c r="R281" t="n">
-        <v>5.03</v>
+        <v>1.84</v>
       </c>
       <c r="S281" t="inlineStr">
         <is>
-          <t>20/10/2023 01:42</t>
+          <t>19/10/2023 23:13</t>
         </is>
       </c>
       <c r="T281" t="n">
-        <v>4.08</v>
+        <v>1.79</v>
       </c>
       <c r="U281" t="inlineStr">
         <is>
@@ -26305,7 +26305,7 @@
       </c>
       <c r="V281" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/corinthians-america-mg/QH6NzSsH/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/coritiba-palmeiras/hSj2Tqzi/</t>
         </is>
       </c>
     </row>
@@ -26609,71 +26609,71 @@
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>Cruzeiro</t>
+          <t>Palmeiras</t>
         </is>
       </c>
       <c r="G285" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H285" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Sao Paulo</t>
         </is>
       </c>
       <c r="I285" t="n">
         <v>0</v>
       </c>
       <c r="J285" t="n">
-        <v>1.92</v>
+        <v>1.75</v>
       </c>
       <c r="K285" t="inlineStr">
         <is>
-          <t>22/10/2023 20:12</t>
+          <t>22/10/2023 22:42</t>
         </is>
       </c>
       <c r="L285" t="n">
-        <v>2</v>
+        <v>2.09</v>
       </c>
       <c r="M285" t="inlineStr">
         <is>
-          <t>26/10/2023 00:54</t>
+          <t>26/10/2023 00:59</t>
         </is>
       </c>
       <c r="N285" t="n">
-        <v>3.59</v>
+        <v>3.78</v>
       </c>
       <c r="O285" t="inlineStr">
         <is>
-          <t>22/10/2023 20:12</t>
+          <t>22/10/2023 22:42</t>
         </is>
       </c>
       <c r="P285" t="n">
-        <v>3.26</v>
+        <v>3.25</v>
       </c>
       <c r="Q285" t="inlineStr">
         <is>
-          <t>26/10/2023 00:54</t>
+          <t>26/10/2023 00:59</t>
         </is>
       </c>
       <c r="R285" t="n">
-        <v>4.3</v>
+        <v>5.03</v>
       </c>
       <c r="S285" t="inlineStr">
         <is>
-          <t>22/10/2023 20:12</t>
+          <t>22/10/2023 22:42</t>
         </is>
       </c>
       <c r="T285" t="n">
-        <v>4.51</v>
+        <v>4.15</v>
       </c>
       <c r="U285" t="inlineStr">
         <is>
-          <t>26/10/2023 00:54</t>
+          <t>26/10/2023 00:59</t>
         </is>
       </c>
       <c r="V285" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/cruzeiro-bahia/E5gZRiGq/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/palmeiras-sao-paulo/4W3aYgwG/</t>
         </is>
       </c>
     </row>
@@ -26701,71 +26701,71 @@
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>Palmeiras</t>
+          <t>Cruzeiro</t>
         </is>
       </c>
       <c r="G286" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H286" t="inlineStr">
         <is>
-          <t>Sao Paulo</t>
+          <t>Bahia</t>
         </is>
       </c>
       <c r="I286" t="n">
         <v>0</v>
       </c>
       <c r="J286" t="n">
-        <v>1.75</v>
+        <v>1.92</v>
       </c>
       <c r="K286" t="inlineStr">
         <is>
-          <t>22/10/2023 22:42</t>
+          <t>22/10/2023 20:12</t>
         </is>
       </c>
       <c r="L286" t="n">
-        <v>2.09</v>
+        <v>2</v>
       </c>
       <c r="M286" t="inlineStr">
         <is>
-          <t>26/10/2023 00:59</t>
+          <t>26/10/2023 00:54</t>
         </is>
       </c>
       <c r="N286" t="n">
-        <v>3.78</v>
+        <v>3.59</v>
       </c>
       <c r="O286" t="inlineStr">
         <is>
-          <t>22/10/2023 22:42</t>
+          <t>22/10/2023 20:12</t>
         </is>
       </c>
       <c r="P286" t="n">
-        <v>3.25</v>
+        <v>3.26</v>
       </c>
       <c r="Q286" t="inlineStr">
         <is>
-          <t>26/10/2023 00:59</t>
+          <t>26/10/2023 00:54</t>
         </is>
       </c>
       <c r="R286" t="n">
-        <v>5.03</v>
+        <v>4.3</v>
       </c>
       <c r="S286" t="inlineStr">
         <is>
-          <t>22/10/2023 22:42</t>
+          <t>22/10/2023 20:12</t>
         </is>
       </c>
       <c r="T286" t="n">
-        <v>4.15</v>
+        <v>4.51</v>
       </c>
       <c r="U286" t="inlineStr">
         <is>
-          <t>26/10/2023 00:59</t>
+          <t>26/10/2023 00:54</t>
         </is>
       </c>
       <c r="V286" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/palmeiras-sao-paulo/4W3aYgwG/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/cruzeiro-bahia/E5gZRiGq/</t>
         </is>
       </c>
     </row>
@@ -26793,71 +26793,71 @@
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Gremio</t>
         </is>
       </c>
       <c r="G287" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H287" t="inlineStr">
         <is>
-          <t>Corinthians</t>
+          <t>Flamengo RJ</t>
         </is>
       </c>
       <c r="I287" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J287" t="n">
+        <v>2.54</v>
+      </c>
+      <c r="K287" t="inlineStr">
+        <is>
+          <t>22/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="L287" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="M287" t="inlineStr">
+        <is>
+          <t>26/10/2023 02:27</t>
+        </is>
+      </c>
+      <c r="N287" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="O287" t="inlineStr">
+        <is>
+          <t>22/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="P287" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="Q287" t="inlineStr">
+        <is>
+          <t>26/10/2023 02:22</t>
+        </is>
+      </c>
+      <c r="R287" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="S287" t="inlineStr">
+        <is>
+          <t>22/10/2023 20:12</t>
+        </is>
+      </c>
+      <c r="T287" t="n">
         <v>2.03</v>
       </c>
-      <c r="K287" t="inlineStr">
-        <is>
-          <t>22/10/2023 22:42</t>
-        </is>
-      </c>
-      <c r="L287" t="n">
-        <v>2.23</v>
-      </c>
-      <c r="M287" t="inlineStr">
-        <is>
-          <t>26/10/2023 02:29</t>
-        </is>
-      </c>
-      <c r="N287" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="O287" t="inlineStr">
-        <is>
-          <t>22/10/2023 22:42</t>
-        </is>
-      </c>
-      <c r="P287" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="Q287" t="inlineStr">
+      <c r="U287" t="inlineStr">
         <is>
           <t>26/10/2023 02:27</t>
         </is>
       </c>
-      <c r="R287" t="n">
-        <v>4.27</v>
-      </c>
-      <c r="S287" t="inlineStr">
-        <is>
-          <t>22/10/2023 22:42</t>
-        </is>
-      </c>
-      <c r="T287" t="n">
-        <v>3.88</v>
-      </c>
-      <c r="U287" t="inlineStr">
-        <is>
-          <t>26/10/2023 02:29</t>
-        </is>
-      </c>
       <c r="V287" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/cuiaba-corinthians/MLgTmZx3/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/gremio-flamengo-rj/WtlvRBVk/</t>
         </is>
       </c>
     </row>
@@ -26885,71 +26885,71 @@
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>Gremio</t>
+          <t>Cuiaba</t>
         </is>
       </c>
       <c r="G288" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H288" t="inlineStr">
         <is>
-          <t>Flamengo RJ</t>
+          <t>Corinthians</t>
         </is>
       </c>
       <c r="I288" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J288" t="n">
-        <v>2.54</v>
+        <v>2.03</v>
       </c>
       <c r="K288" t="inlineStr">
         <is>
-          <t>22/10/2023 20:12</t>
+          <t>22/10/2023 22:42</t>
         </is>
       </c>
       <c r="L288" t="n">
-        <v>4.14</v>
+        <v>2.23</v>
       </c>
       <c r="M288" t="inlineStr">
         <is>
+          <t>26/10/2023 02:29</t>
+        </is>
+      </c>
+      <c r="N288" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="O288" t="inlineStr">
+        <is>
+          <t>22/10/2023 22:42</t>
+        </is>
+      </c>
+      <c r="P288" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="Q288" t="inlineStr">
+        <is>
           <t>26/10/2023 02:27</t>
         </is>
       </c>
-      <c r="N288" t="n">
-        <v>3.37</v>
-      </c>
-      <c r="O288" t="inlineStr">
-        <is>
-          <t>22/10/2023 20:12</t>
-        </is>
-      </c>
-      <c r="P288" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="Q288" t="inlineStr">
-        <is>
-          <t>26/10/2023 02:22</t>
-        </is>
-      </c>
       <c r="R288" t="n">
-        <v>2.93</v>
+        <v>4.27</v>
       </c>
       <c r="S288" t="inlineStr">
         <is>
-          <t>22/10/2023 20:12</t>
+          <t>22/10/2023 22:42</t>
         </is>
       </c>
       <c r="T288" t="n">
-        <v>2.03</v>
+        <v>3.88</v>
       </c>
       <c r="U288" t="inlineStr">
         <is>
-          <t>26/10/2023 02:27</t>
+          <t>26/10/2023 02:29</t>
         </is>
       </c>
       <c r="V288" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/gremio-flamengo-rj/WtlvRBVk/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/cuiaba-corinthians/MLgTmZx3/</t>
         </is>
       </c>
     </row>
@@ -27989,7 +27989,7 @@
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>Internacional</t>
+          <t>Corinthians</t>
         </is>
       </c>
       <c r="G300" t="n">
@@ -27997,14 +27997,14 @@
       </c>
       <c r="H300" t="inlineStr">
         <is>
-          <t>America MG</t>
+          <t>Athletico-PR</t>
         </is>
       </c>
       <c r="I300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J300" t="n">
-        <v>1.65</v>
+        <v>2.7</v>
       </c>
       <c r="K300" t="inlineStr">
         <is>
@@ -28012,15 +28012,15 @@
         </is>
       </c>
       <c r="L300" t="n">
-        <v>1.58</v>
+        <v>2.73</v>
       </c>
       <c r="M300" t="inlineStr">
         <is>
-          <t>01/11/2023 22:58</t>
+          <t>01/11/2023 22:51</t>
         </is>
       </c>
       <c r="N300" t="n">
-        <v>4.12</v>
+        <v>3.14</v>
       </c>
       <c r="O300" t="inlineStr">
         <is>
@@ -28028,15 +28028,15 @@
         </is>
       </c>
       <c r="P300" t="n">
-        <v>4.38</v>
+        <v>3</v>
       </c>
       <c r="Q300" t="inlineStr">
         <is>
-          <t>01/11/2023 22:58</t>
+          <t>01/11/2023 22:50</t>
         </is>
       </c>
       <c r="R300" t="n">
-        <v>5.2</v>
+        <v>2.86</v>
       </c>
       <c r="S300" t="inlineStr">
         <is>
@@ -28044,16 +28044,16 @@
         </is>
       </c>
       <c r="T300" t="n">
-        <v>5.87</v>
+        <v>3.05</v>
       </c>
       <c r="U300" t="inlineStr">
         <is>
-          <t>01/11/2023 22:58</t>
+          <t>01/11/2023 22:51</t>
         </is>
       </c>
       <c r="V300" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/internacional-america-mg/4U2ejSb1/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/corinthians-athletico-pr/EuArgUEr/</t>
         </is>
       </c>
     </row>
@@ -28081,7 +28081,7 @@
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>Corinthians</t>
+          <t>Internacional</t>
         </is>
       </c>
       <c r="G301" t="n">
@@ -28089,14 +28089,14 @@
       </c>
       <c r="H301" t="inlineStr">
         <is>
-          <t>Athletico-PR</t>
+          <t>America MG</t>
         </is>
       </c>
       <c r="I301" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J301" t="n">
-        <v>2.7</v>
+        <v>1.65</v>
       </c>
       <c r="K301" t="inlineStr">
         <is>
@@ -28104,15 +28104,15 @@
         </is>
       </c>
       <c r="L301" t="n">
-        <v>2.73</v>
+        <v>1.58</v>
       </c>
       <c r="M301" t="inlineStr">
         <is>
-          <t>01/11/2023 22:51</t>
+          <t>01/11/2023 22:58</t>
         </is>
       </c>
       <c r="N301" t="n">
-        <v>3.14</v>
+        <v>4.12</v>
       </c>
       <c r="O301" t="inlineStr">
         <is>
@@ -28120,15 +28120,15 @@
         </is>
       </c>
       <c r="P301" t="n">
-        <v>3</v>
+        <v>4.38</v>
       </c>
       <c r="Q301" t="inlineStr">
         <is>
-          <t>01/11/2023 22:50</t>
+          <t>01/11/2023 22:58</t>
         </is>
       </c>
       <c r="R301" t="n">
-        <v>2.86</v>
+        <v>5.2</v>
       </c>
       <c r="S301" t="inlineStr">
         <is>
@@ -28136,16 +28136,16 @@
         </is>
       </c>
       <c r="T301" t="n">
-        <v>3.05</v>
+        <v>5.87</v>
       </c>
       <c r="U301" t="inlineStr">
         <is>
-          <t>01/11/2023 22:51</t>
+          <t>01/11/2023 22:58</t>
         </is>
       </c>
       <c r="V301" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/corinthians-athletico-pr/EuArgUEr/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/internacional-america-mg/4U2ejSb1/</t>
         </is>
       </c>
     </row>
@@ -28173,7 +28173,7 @@
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>Coritiba</t>
+          <t>Flamengo RJ</t>
         </is>
       </c>
       <c r="G302" t="n">
@@ -28181,14 +28181,14 @@
       </c>
       <c r="H302" t="inlineStr">
         <is>
-          <t>Gremio</t>
+          <t>Santos</t>
         </is>
       </c>
       <c r="I302" t="n">
         <v>2</v>
       </c>
       <c r="J302" t="n">
-        <v>3.13</v>
+        <v>1.38</v>
       </c>
       <c r="K302" t="inlineStr">
         <is>
@@ -28196,15 +28196,15 @@
         </is>
       </c>
       <c r="L302" t="n">
-        <v>3.22</v>
+        <v>1.47</v>
       </c>
       <c r="M302" t="inlineStr">
         <is>
-          <t>01/11/2023 23:58</t>
+          <t>01/11/2023 23:55</t>
         </is>
       </c>
       <c r="N302" t="n">
-        <v>3.37</v>
+        <v>5.05</v>
       </c>
       <c r="O302" t="inlineStr">
         <is>
@@ -28212,15 +28212,15 @@
         </is>
       </c>
       <c r="P302" t="n">
-        <v>3.68</v>
+        <v>4.52</v>
       </c>
       <c r="Q302" t="inlineStr">
         <is>
-          <t>01/11/2023 23:58</t>
+          <t>01/11/2023 23:59</t>
         </is>
       </c>
       <c r="R302" t="n">
-        <v>2.36</v>
+        <v>8.69</v>
       </c>
       <c r="S302" t="inlineStr">
         <is>
@@ -28228,16 +28228,16 @@
         </is>
       </c>
       <c r="T302" t="n">
-        <v>2.24</v>
+        <v>7.59</v>
       </c>
       <c r="U302" t="inlineStr">
         <is>
-          <t>01/11/2023 23:58</t>
+          <t>01/11/2023 23:57</t>
         </is>
       </c>
       <c r="V302" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/coritiba-gremio/G46aknE7/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/flamengo-rj-santos/G4U7aWyF/</t>
         </is>
       </c>
     </row>
@@ -28265,7 +28265,7 @@
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>Flamengo RJ</t>
+          <t>Coritiba</t>
         </is>
       </c>
       <c r="G303" t="n">
@@ -28273,14 +28273,14 @@
       </c>
       <c r="H303" t="inlineStr">
         <is>
-          <t>Santos</t>
+          <t>Gremio</t>
         </is>
       </c>
       <c r="I303" t="n">
         <v>2</v>
       </c>
       <c r="J303" t="n">
-        <v>1.38</v>
+        <v>3.13</v>
       </c>
       <c r="K303" t="inlineStr">
         <is>
@@ -28288,15 +28288,15 @@
         </is>
       </c>
       <c r="L303" t="n">
-        <v>1.47</v>
+        <v>3.22</v>
       </c>
       <c r="M303" t="inlineStr">
         <is>
-          <t>01/11/2023 23:55</t>
+          <t>01/11/2023 23:58</t>
         </is>
       </c>
       <c r="N303" t="n">
-        <v>5.05</v>
+        <v>3.37</v>
       </c>
       <c r="O303" t="inlineStr">
         <is>
@@ -28304,15 +28304,15 @@
         </is>
       </c>
       <c r="P303" t="n">
-        <v>4.52</v>
+        <v>3.68</v>
       </c>
       <c r="Q303" t="inlineStr">
         <is>
-          <t>01/11/2023 23:59</t>
+          <t>01/11/2023 23:58</t>
         </is>
       </c>
       <c r="R303" t="n">
-        <v>8.69</v>
+        <v>2.36</v>
       </c>
       <c r="S303" t="inlineStr">
         <is>
@@ -28320,16 +28320,16 @@
         </is>
       </c>
       <c r="T303" t="n">
-        <v>7.59</v>
+        <v>2.24</v>
       </c>
       <c r="U303" t="inlineStr">
         <is>
-          <t>01/11/2023 23:57</t>
+          <t>01/11/2023 23:58</t>
         </is>
       </c>
       <c r="V303" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/flamengo-rj-santos/G4U7aWyF/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/coritiba-gremio/G46aknE7/</t>
         </is>
       </c>
     </row>
@@ -29093,71 +29093,71 @@
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>Cruzeiro</t>
+          <t>Fortaleza</t>
         </is>
       </c>
       <c r="G312" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H312" t="inlineStr">
         <is>
-          <t>Internacional</t>
+          <t>Flamengo RJ</t>
         </is>
       </c>
       <c r="I312" t="n">
         <v>2</v>
       </c>
       <c r="J312" t="n">
-        <v>2.14</v>
+        <v>2.84</v>
       </c>
       <c r="K312" t="inlineStr">
         <is>
-          <t>03/11/2023 00:12</t>
+          <t>02/11/2023 01:42</t>
         </is>
       </c>
       <c r="L312" t="n">
-        <v>2.21</v>
+        <v>2.58</v>
       </c>
       <c r="M312" t="inlineStr">
         <is>
-          <t>05/11/2023 19:57</t>
+          <t>05/11/2023 19:58</t>
         </is>
       </c>
       <c r="N312" t="n">
-        <v>3.34</v>
+        <v>3.27</v>
       </c>
       <c r="O312" t="inlineStr">
         <is>
-          <t>03/11/2023 00:12</t>
+          <t>02/11/2023 01:42</t>
         </is>
       </c>
       <c r="P312" t="n">
-        <v>3.06</v>
+        <v>3.16</v>
       </c>
       <c r="Q312" t="inlineStr">
         <is>
-          <t>05/11/2023 19:59</t>
+          <t>05/11/2023 19:52</t>
         </is>
       </c>
       <c r="R312" t="n">
-        <v>3.76</v>
+        <v>2.63</v>
       </c>
       <c r="S312" t="inlineStr">
         <is>
-          <t>03/11/2023 00:12</t>
+          <t>02/11/2023 01:42</t>
         </is>
       </c>
       <c r="T312" t="n">
-        <v>4.02</v>
+        <v>3.09</v>
       </c>
       <c r="U312" t="inlineStr">
         <is>
-          <t>05/11/2023 19:57</t>
+          <t>05/11/2023 19:58</t>
         </is>
       </c>
       <c r="V312" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/cruzeiro-internacional/Wv3ziakC/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/fortaleza-flamengo-rj/6BfQDMdP/</t>
         </is>
       </c>
     </row>
@@ -29185,7 +29185,7 @@
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>Bragantino</t>
+          <t>Cruzeiro</t>
         </is>
       </c>
       <c r="G313" t="n">
@@ -29193,54 +29193,54 @@
       </c>
       <c r="H313" t="inlineStr">
         <is>
-          <t>Corinthians</t>
+          <t>Internacional</t>
         </is>
       </c>
       <c r="I313" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J313" t="n">
-        <v>1.58</v>
+        <v>2.14</v>
       </c>
       <c r="K313" t="inlineStr">
         <is>
-          <t>02/11/2023 22:12</t>
+          <t>03/11/2023 00:12</t>
         </is>
       </c>
       <c r="L313" t="n">
-        <v>1.6</v>
+        <v>2.21</v>
       </c>
       <c r="M313" t="inlineStr">
         <is>
-          <t>05/11/2023 19:53</t>
+          <t>05/11/2023 19:57</t>
         </is>
       </c>
       <c r="N313" t="n">
-        <v>4.08</v>
+        <v>3.34</v>
       </c>
       <c r="O313" t="inlineStr">
         <is>
-          <t>02/11/2023 22:12</t>
+          <t>03/11/2023 00:12</t>
         </is>
       </c>
       <c r="P313" t="n">
-        <v>4.22</v>
+        <v>3.06</v>
       </c>
       <c r="Q313" t="inlineStr">
         <is>
-          <t>05/11/2023 19:58</t>
+          <t>05/11/2023 19:59</t>
         </is>
       </c>
       <c r="R313" t="n">
-        <v>6.35</v>
+        <v>3.76</v>
       </c>
       <c r="S313" t="inlineStr">
         <is>
-          <t>02/11/2023 22:12</t>
+          <t>03/11/2023 00:12</t>
         </is>
       </c>
       <c r="T313" t="n">
-        <v>5.87</v>
+        <v>4.02</v>
       </c>
       <c r="U313" t="inlineStr">
         <is>
@@ -29249,7 +29249,7 @@
       </c>
       <c r="V313" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/bragantino-corinthians/hl4Wiuz6/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/cruzeiro-internacional/Wv3ziakC/</t>
         </is>
       </c>
     </row>
@@ -29277,71 +29277,71 @@
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Bragantino</t>
         </is>
       </c>
       <c r="G314" t="n">
+        <v>1</v>
+      </c>
+      <c r="H314" t="inlineStr">
+        <is>
+          <t>Corinthians</t>
+        </is>
+      </c>
+      <c r="I314" t="n">
         <v>0</v>
       </c>
-      <c r="H314" t="inlineStr">
-        <is>
-          <t>Flamengo RJ</t>
-        </is>
-      </c>
-      <c r="I314" t="n">
-        <v>2</v>
-      </c>
       <c r="J314" t="n">
-        <v>2.84</v>
+        <v>1.58</v>
       </c>
       <c r="K314" t="inlineStr">
         <is>
-          <t>02/11/2023 01:42</t>
+          <t>02/11/2023 22:12</t>
         </is>
       </c>
       <c r="L314" t="n">
-        <v>2.58</v>
+        <v>1.6</v>
       </c>
       <c r="M314" t="inlineStr">
         <is>
+          <t>05/11/2023 19:53</t>
+        </is>
+      </c>
+      <c r="N314" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="O314" t="inlineStr">
+        <is>
+          <t>02/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P314" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="Q314" t="inlineStr">
+        <is>
           <t>05/11/2023 19:58</t>
         </is>
       </c>
-      <c r="N314" t="n">
-        <v>3.27</v>
-      </c>
-      <c r="O314" t="inlineStr">
-        <is>
-          <t>02/11/2023 01:42</t>
-        </is>
-      </c>
-      <c r="P314" t="n">
-        <v>3.16</v>
-      </c>
-      <c r="Q314" t="inlineStr">
-        <is>
-          <t>05/11/2023 19:52</t>
-        </is>
-      </c>
       <c r="R314" t="n">
-        <v>2.63</v>
+        <v>6.35</v>
       </c>
       <c r="S314" t="inlineStr">
         <is>
-          <t>02/11/2023 01:42</t>
+          <t>02/11/2023 22:12</t>
         </is>
       </c>
       <c r="T314" t="n">
-        <v>3.09</v>
+        <v>5.87</v>
       </c>
       <c r="U314" t="inlineStr">
         <is>
-          <t>05/11/2023 19:58</t>
+          <t>05/11/2023 19:57</t>
         </is>
       </c>
       <c r="V314" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/fortaleza-flamengo-rj/6BfQDMdP/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/bragantino-corinthians/hl4Wiuz6/</t>
         </is>
       </c>
     </row>
@@ -30289,71 +30289,71 @@
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>Botafogo RJ</t>
+          <t>Bahia</t>
         </is>
       </c>
       <c r="G325" t="n">
+        <v>0</v>
+      </c>
+      <c r="H325" t="inlineStr">
+        <is>
+          <t>Cuiaba</t>
+        </is>
+      </c>
+      <c r="I325" t="n">
         <v>3</v>
       </c>
-      <c r="H325" t="inlineStr">
-        <is>
-          <t>Gremio</t>
-        </is>
-      </c>
-      <c r="I325" t="n">
-        <v>4</v>
-      </c>
       <c r="J325" t="n">
-        <v>1.82</v>
+        <v>1.79</v>
       </c>
       <c r="K325" t="inlineStr">
         <is>
-          <t>06/11/2023 23:12</t>
+          <t>07/11/2023 01:12</t>
         </is>
       </c>
       <c r="L325" t="n">
-        <v>1.95</v>
+        <v>1.86</v>
       </c>
       <c r="M325" t="inlineStr">
         <is>
-          <t>09/11/2023 23:59</t>
+          <t>09/11/2023 23:30</t>
         </is>
       </c>
       <c r="N325" t="n">
-        <v>3.75</v>
+        <v>3.61</v>
       </c>
       <c r="O325" t="inlineStr">
         <is>
-          <t>06/11/2023 23:12</t>
+          <t>07/11/2023 01:12</t>
         </is>
       </c>
       <c r="P325" t="n">
-        <v>3.71</v>
+        <v>3.45</v>
       </c>
       <c r="Q325" t="inlineStr">
         <is>
-          <t>09/11/2023 23:59</t>
+          <t>09/11/2023 23:30</t>
         </is>
       </c>
       <c r="R325" t="n">
-        <v>4.46</v>
+        <v>4.8</v>
       </c>
       <c r="S325" t="inlineStr">
         <is>
-          <t>06/11/2023 23:12</t>
+          <t>07/11/2023 01:12</t>
         </is>
       </c>
       <c r="T325" t="n">
-        <v>4.03</v>
+        <v>4.93</v>
       </c>
       <c r="U325" t="inlineStr">
         <is>
-          <t>09/11/2023 23:59</t>
+          <t>09/11/2023 23:30</t>
         </is>
       </c>
       <c r="V325" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/botafogo-rj-gremio/Gpp07KZh/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/bahia-cuiaba/jcBVMaZu/</t>
         </is>
       </c>
     </row>
@@ -30381,71 +30381,71 @@
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Botafogo RJ</t>
         </is>
       </c>
       <c r="G326" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H326" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Gremio</t>
         </is>
       </c>
       <c r="I326" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J326" t="n">
-        <v>1.79</v>
+        <v>1.82</v>
       </c>
       <c r="K326" t="inlineStr">
         <is>
-          <t>07/11/2023 01:12</t>
+          <t>06/11/2023 23:12</t>
         </is>
       </c>
       <c r="L326" t="n">
-        <v>1.86</v>
+        <v>1.95</v>
       </c>
       <c r="M326" t="inlineStr">
         <is>
-          <t>09/11/2023 23:30</t>
+          <t>09/11/2023 23:59</t>
         </is>
       </c>
       <c r="N326" t="n">
-        <v>3.61</v>
+        <v>3.75</v>
       </c>
       <c r="O326" t="inlineStr">
         <is>
-          <t>07/11/2023 01:12</t>
+          <t>06/11/2023 23:12</t>
         </is>
       </c>
       <c r="P326" t="n">
-        <v>3.45</v>
+        <v>3.71</v>
       </c>
       <c r="Q326" t="inlineStr">
         <is>
-          <t>09/11/2023 23:30</t>
+          <t>09/11/2023 23:59</t>
         </is>
       </c>
       <c r="R326" t="n">
-        <v>4.8</v>
+        <v>4.46</v>
       </c>
       <c r="S326" t="inlineStr">
         <is>
-          <t>07/11/2023 01:12</t>
+          <t>06/11/2023 23:12</t>
         </is>
       </c>
       <c r="T326" t="n">
-        <v>4.93</v>
+        <v>4.03</v>
       </c>
       <c r="U326" t="inlineStr">
         <is>
-          <t>09/11/2023 23:30</t>
+          <t>09/11/2023 23:59</t>
         </is>
       </c>
       <c r="V326" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/bahia-cuiaba/jcBVMaZu/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/botafogo-rj-gremio/Gpp07KZh/</t>
         </is>
       </c>
     </row>
@@ -31117,71 +31117,71 @@
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Atletico-MG</t>
         </is>
       </c>
       <c r="G334" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H334" t="inlineStr">
         <is>
-          <t>Athletico-PR</t>
+          <t>Goias</t>
         </is>
       </c>
       <c r="I334" t="n">
         <v>1</v>
       </c>
       <c r="J334" t="n">
-        <v>2.29</v>
+        <v>1.58</v>
       </c>
       <c r="K334" t="inlineStr">
         <is>
-          <t>09/11/2023 09:03</t>
+          <t>09/11/2023 09:02</t>
         </is>
       </c>
       <c r="L334" t="n">
-        <v>2.3</v>
+        <v>1.59</v>
       </c>
       <c r="M334" t="inlineStr">
         <is>
-          <t>12/11/2023 22:27</t>
+          <t>12/11/2023 22:28</t>
         </is>
       </c>
       <c r="N334" t="n">
-        <v>3.21</v>
+        <v>4</v>
       </c>
       <c r="O334" t="inlineStr">
         <is>
-          <t>09/11/2023 09:03</t>
+          <t>09/11/2023 09:02</t>
         </is>
       </c>
       <c r="P334" t="n">
-        <v>3.31</v>
+        <v>3.91</v>
       </c>
       <c r="Q334" t="inlineStr">
         <is>
+          <t>12/11/2023 22:11</t>
+        </is>
+      </c>
+      <c r="R334" t="n">
+        <v>6.21</v>
+      </c>
+      <c r="S334" t="inlineStr">
+        <is>
+          <t>09/11/2023 09:02</t>
+        </is>
+      </c>
+      <c r="T334" t="n">
+        <v>6.91</v>
+      </c>
+      <c r="U334" t="inlineStr">
+        <is>
           <t>12/11/2023 22:28</t>
         </is>
       </c>
-      <c r="R334" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="S334" t="inlineStr">
-        <is>
-          <t>09/11/2023 09:03</t>
-        </is>
-      </c>
-      <c r="T334" t="n">
-        <v>3.44</v>
-      </c>
-      <c r="U334" t="inlineStr">
-        <is>
-          <t>12/11/2023 22:28</t>
-        </is>
-      </c>
       <c r="V334" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/bahia-athletico-pr/jJn6ZxJo/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/atletico-mg-goias/IVHiGFIN/</t>
         </is>
       </c>
     </row>
@@ -31209,62 +31209,62 @@
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>Atletico-MG</t>
+          <t>Bahia</t>
         </is>
       </c>
       <c r="G335" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H335" t="inlineStr">
         <is>
-          <t>Goias</t>
+          <t>Athletico-PR</t>
         </is>
       </c>
       <c r="I335" t="n">
         <v>1</v>
       </c>
       <c r="J335" t="n">
-        <v>1.58</v>
+        <v>2.29</v>
       </c>
       <c r="K335" t="inlineStr">
         <is>
-          <t>09/11/2023 09:02</t>
+          <t>09/11/2023 09:03</t>
         </is>
       </c>
       <c r="L335" t="n">
-        <v>1.59</v>
+        <v>2.3</v>
       </c>
       <c r="M335" t="inlineStr">
         <is>
+          <t>12/11/2023 22:27</t>
+        </is>
+      </c>
+      <c r="N335" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="O335" t="inlineStr">
+        <is>
+          <t>09/11/2023 09:03</t>
+        </is>
+      </c>
+      <c r="P335" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="Q335" t="inlineStr">
+        <is>
           <t>12/11/2023 22:28</t>
         </is>
       </c>
-      <c r="N335" t="n">
-        <v>4</v>
-      </c>
-      <c r="O335" t="inlineStr">
-        <is>
-          <t>09/11/2023 09:02</t>
-        </is>
-      </c>
-      <c r="P335" t="n">
-        <v>3.91</v>
-      </c>
-      <c r="Q335" t="inlineStr">
-        <is>
-          <t>12/11/2023 22:11</t>
-        </is>
-      </c>
       <c r="R335" t="n">
-        <v>6.21</v>
+        <v>3.45</v>
       </c>
       <c r="S335" t="inlineStr">
         <is>
-          <t>09/11/2023 09:02</t>
+          <t>09/11/2023 09:03</t>
         </is>
       </c>
       <c r="T335" t="n">
-        <v>6.91</v>
+        <v>3.44</v>
       </c>
       <c r="U335" t="inlineStr">
         <is>
@@ -31273,7 +31273,7 @@
       </c>
       <c r="V335" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/atletico-mg-goias/IVHiGFIN/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/bahia-athletico-pr/jJn6ZxJo/</t>
         </is>
       </c>
     </row>
@@ -32129,71 +32129,71 @@
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>Botafogo RJ</t>
+          <t>Atletico-MG</t>
         </is>
       </c>
       <c r="G345" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H345" t="inlineStr">
         <is>
-          <t>Santos</t>
+          <t>Gremio</t>
         </is>
       </c>
       <c r="I345" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J345" t="n">
         <v>1.69</v>
       </c>
       <c r="K345" t="inlineStr">
         <is>
-          <t>23/11/2023 23:12</t>
+          <t>12/11/2023 22:42</t>
         </is>
       </c>
       <c r="L345" t="n">
-        <v>1.84</v>
+        <v>1.77</v>
       </c>
       <c r="M345" t="inlineStr">
         <is>
-          <t>26/11/2023 19:59</t>
+          <t>26/11/2023 19:58</t>
         </is>
       </c>
       <c r="N345" t="n">
-        <v>3.85</v>
+        <v>3.91</v>
       </c>
       <c r="O345" t="inlineStr">
         <is>
-          <t>23/11/2023 23:12</t>
+          <t>12/11/2023 22:42</t>
         </is>
       </c>
       <c r="P345" t="n">
-        <v>3.55</v>
+        <v>3.75</v>
       </c>
       <c r="Q345" t="inlineStr">
         <is>
-          <t>26/11/2023 19:57</t>
+          <t>26/11/2023 19:58</t>
         </is>
       </c>
       <c r="R345" t="n">
-        <v>5.45</v>
+        <v>5.32</v>
       </c>
       <c r="S345" t="inlineStr">
         <is>
-          <t>23/11/2023 23:12</t>
+          <t>12/11/2023 22:42</t>
         </is>
       </c>
       <c r="T345" t="n">
-        <v>4.89</v>
+        <v>5.05</v>
       </c>
       <c r="U345" t="inlineStr">
         <is>
-          <t>26/11/2023 19:59</t>
+          <t>26/11/2023 19:58</t>
         </is>
       </c>
       <c r="V345" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/botafogo-rj-santos/xzkIWz34/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/atletico-mg-gremio/jceYSh2T/</t>
         </is>
       </c>
     </row>
@@ -32221,71 +32221,71 @@
       </c>
       <c r="F346" t="inlineStr">
         <is>
-          <t>Atletico-MG</t>
+          <t>Botafogo RJ</t>
         </is>
       </c>
       <c r="G346" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H346" t="inlineStr">
         <is>
-          <t>Gremio</t>
+          <t>Santos</t>
         </is>
       </c>
       <c r="I346" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J346" t="n">
         <v>1.69</v>
       </c>
       <c r="K346" t="inlineStr">
         <is>
-          <t>12/11/2023 22:42</t>
+          <t>23/11/2023 23:12</t>
         </is>
       </c>
       <c r="L346" t="n">
-        <v>1.77</v>
+        <v>1.84</v>
       </c>
       <c r="M346" t="inlineStr">
         <is>
-          <t>26/11/2023 19:58</t>
+          <t>26/11/2023 19:59</t>
         </is>
       </c>
       <c r="N346" t="n">
-        <v>3.91</v>
+        <v>3.85</v>
       </c>
       <c r="O346" t="inlineStr">
         <is>
-          <t>12/11/2023 22:42</t>
+          <t>23/11/2023 23:12</t>
         </is>
       </c>
       <c r="P346" t="n">
-        <v>3.75</v>
+        <v>3.55</v>
       </c>
       <c r="Q346" t="inlineStr">
         <is>
-          <t>26/11/2023 19:58</t>
+          <t>26/11/2023 19:57</t>
         </is>
       </c>
       <c r="R346" t="n">
-        <v>5.32</v>
+        <v>5.45</v>
       </c>
       <c r="S346" t="inlineStr">
         <is>
-          <t>12/11/2023 22:42</t>
+          <t>23/11/2023 23:12</t>
         </is>
       </c>
       <c r="T346" t="n">
-        <v>5.05</v>
+        <v>4.89</v>
       </c>
       <c r="U346" t="inlineStr">
         <is>
-          <t>26/11/2023 19:58</t>
+          <t>26/11/2023 19:59</t>
         </is>
       </c>
       <c r="V346" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/atletico-mg-gremio/jceYSh2T/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/botafogo-rj-santos/xzkIWz34/</t>
         </is>
       </c>
     </row>
@@ -32405,7 +32405,7 @@
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>Sao Paulo</t>
+          <t>America MG</t>
         </is>
       </c>
       <c r="G348" t="n">
@@ -32413,63 +32413,63 @@
       </c>
       <c r="H348" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Flamengo RJ</t>
         </is>
       </c>
       <c r="I348" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J348" t="n">
-        <v>1.65</v>
+        <v>6.15</v>
       </c>
       <c r="K348" t="inlineStr">
         <is>
-          <t>23/11/2023 01:42</t>
+          <t>24/11/2023 01:42</t>
         </is>
       </c>
       <c r="L348" t="n">
-        <v>1.7</v>
+        <v>8.52</v>
       </c>
       <c r="M348" t="inlineStr">
         <is>
-          <t>26/11/2023 22:01</t>
+          <t>26/11/2023 22:06</t>
         </is>
       </c>
       <c r="N348" t="n">
-        <v>3.75</v>
+        <v>4.5</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
-          <t>23/11/2023 01:42</t>
+          <t>24/11/2023 01:42</t>
         </is>
       </c>
       <c r="P348" t="n">
-        <v>3.5</v>
+        <v>5.02</v>
       </c>
       <c r="Q348" t="inlineStr">
         <is>
-          <t>26/11/2023 22:04</t>
+          <t>26/11/2023 22:06</t>
         </is>
       </c>
       <c r="R348" t="n">
-        <v>6.1</v>
+        <v>1.52</v>
       </c>
       <c r="S348" t="inlineStr">
         <is>
-          <t>23/11/2023 01:42</t>
+          <t>24/11/2023 01:42</t>
         </is>
       </c>
       <c r="T348" t="n">
-        <v>6.32</v>
+        <v>1.4</v>
       </c>
       <c r="U348" t="inlineStr">
         <is>
-          <t>26/11/2023 22:04</t>
+          <t>26/11/2023 22:05</t>
         </is>
       </c>
       <c r="V348" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/sao-paulo-cuiaba/KbvNVfIA/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/america-mg-flamengo-rj/xlUjozIc/</t>
         </is>
       </c>
     </row>
@@ -32497,71 +32497,71 @@
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>America MG</t>
+          <t>Fortaleza</t>
         </is>
       </c>
       <c r="G349" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H349" t="inlineStr">
         <is>
-          <t>Flamengo RJ</t>
+          <t>Palmeiras</t>
         </is>
       </c>
       <c r="I349" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J349" t="n">
-        <v>6.15</v>
+        <v>3.53</v>
       </c>
       <c r="K349" t="inlineStr">
         <is>
-          <t>24/11/2023 01:42</t>
+          <t>23/11/2023 23:12</t>
         </is>
       </c>
       <c r="L349" t="n">
-        <v>8.52</v>
+        <v>3.22</v>
       </c>
       <c r="M349" t="inlineStr">
         <is>
-          <t>26/11/2023 22:06</t>
+          <t>26/11/2023 22:28</t>
         </is>
       </c>
       <c r="N349" t="n">
-        <v>4.5</v>
+        <v>3.31</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
-          <t>24/11/2023 01:42</t>
+          <t>23/11/2023 23:12</t>
         </is>
       </c>
       <c r="P349" t="n">
-        <v>5.02</v>
+        <v>3.22</v>
       </c>
       <c r="Q349" t="inlineStr">
         <is>
-          <t>26/11/2023 22:06</t>
+          <t>26/11/2023 22:28</t>
         </is>
       </c>
       <c r="R349" t="n">
-        <v>1.52</v>
+        <v>2.2</v>
       </c>
       <c r="S349" t="inlineStr">
         <is>
-          <t>24/11/2023 01:42</t>
+          <t>23/11/2023 23:12</t>
         </is>
       </c>
       <c r="T349" t="n">
-        <v>1.4</v>
+        <v>2.46</v>
       </c>
       <c r="U349" t="inlineStr">
         <is>
-          <t>26/11/2023 22:05</t>
+          <t>26/11/2023 22:28</t>
         </is>
       </c>
       <c r="V349" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/america-mg-flamengo-rj/xlUjozIc/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/fortaleza-palmeiras/OpQnnG2i/</t>
         </is>
       </c>
     </row>
@@ -32589,71 +32589,71 @@
       </c>
       <c r="F350" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Sao Paulo</t>
         </is>
       </c>
       <c r="G350" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H350" t="inlineStr">
         <is>
-          <t>Palmeiras</t>
+          <t>Cuiaba</t>
         </is>
       </c>
       <c r="I350" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J350" t="n">
-        <v>3.53</v>
+        <v>1.65</v>
       </c>
       <c r="K350" t="inlineStr">
         <is>
-          <t>23/11/2023 23:12</t>
+          <t>23/11/2023 01:42</t>
         </is>
       </c>
       <c r="L350" t="n">
-        <v>3.22</v>
+        <v>1.7</v>
       </c>
       <c r="M350" t="inlineStr">
         <is>
-          <t>26/11/2023 22:28</t>
+          <t>26/11/2023 22:01</t>
         </is>
       </c>
       <c r="N350" t="n">
-        <v>3.31</v>
+        <v>3.75</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
-          <t>23/11/2023 23:12</t>
+          <t>23/11/2023 01:42</t>
         </is>
       </c>
       <c r="P350" t="n">
-        <v>3.22</v>
+        <v>3.5</v>
       </c>
       <c r="Q350" t="inlineStr">
         <is>
-          <t>26/11/2023 22:28</t>
+          <t>26/11/2023 22:04</t>
         </is>
       </c>
       <c r="R350" t="n">
-        <v>2.2</v>
+        <v>6.1</v>
       </c>
       <c r="S350" t="inlineStr">
         <is>
-          <t>23/11/2023 23:12</t>
+          <t>23/11/2023 01:42</t>
         </is>
       </c>
       <c r="T350" t="n">
-        <v>2.46</v>
+        <v>6.32</v>
       </c>
       <c r="U350" t="inlineStr">
         <is>
-          <t>26/11/2023 22:28</t>
+          <t>26/11/2023 22:04</t>
         </is>
       </c>
       <c r="V350" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/brazil/serie-a/fortaleza-palmeiras/OpQnnG2i/</t>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/sao-paulo-cuiaba/KbvNVfIA/</t>
         </is>
       </c>
     </row>
@@ -32746,6 +32746,98 @@
       <c r="V351" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/brazil/serie-a/goias-cruzeiro/C6dUTYnN/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="1" t="n">
+        <v>351</v>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>brazil</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>serie-a</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E352" s="2" t="n">
+        <v>45259.0625</v>
+      </c>
+      <c r="F352" t="inlineStr">
+        <is>
+          <t>Vasco</t>
+        </is>
+      </c>
+      <c r="G352" t="n">
+        <v>2</v>
+      </c>
+      <c r="H352" t="inlineStr">
+        <is>
+          <t>Corinthians</t>
+        </is>
+      </c>
+      <c r="I352" t="n">
+        <v>4</v>
+      </c>
+      <c r="J352" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="K352" t="inlineStr">
+        <is>
+          <t>25/11/2023 23:42</t>
+        </is>
+      </c>
+      <c r="L352" t="n">
+        <v>2</v>
+      </c>
+      <c r="M352" t="inlineStr">
+        <is>
+          <t>29/11/2023 01:27</t>
+        </is>
+      </c>
+      <c r="N352" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="O352" t="inlineStr">
+        <is>
+          <t>25/11/2023 23:42</t>
+        </is>
+      </c>
+      <c r="P352" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="Q352" t="inlineStr">
+        <is>
+          <t>29/11/2023 01:28</t>
+        </is>
+      </c>
+      <c r="R352" t="n">
+        <v>5.16</v>
+      </c>
+      <c r="S352" t="inlineStr">
+        <is>
+          <t>25/11/2023 23:42</t>
+        </is>
+      </c>
+      <c r="T352" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="U352" t="inlineStr">
+        <is>
+          <t>29/11/2023 01:27</t>
+        </is>
+      </c>
+      <c r="V352" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/brazil/serie-a/vasco-corinthians/b3IaqEnA/</t>
         </is>
       </c>
     </row>

</xml_diff>